<commit_message>
Optimización de las pages y creación de nuevas features
</commit_message>
<xml_diff>
--- a/TestFiles/usersDataset.xlsx
+++ b/TestFiles/usersDataset.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="190">
   <si>
     <t>email</t>
   </si>
@@ -319,6 +319,282 @@
   </si>
   <si>
     <t>87637</t>
+  </si>
+  <si>
+    <t>3RWWKEG0@testmail.com</t>
+  </si>
+  <si>
+    <t>84851</t>
+  </si>
+  <si>
+    <t>1903615730</t>
+  </si>
+  <si>
+    <t>22883</t>
+  </si>
+  <si>
+    <t>PIM9N83O@testmail.com</t>
+  </si>
+  <si>
+    <t>20153</t>
+  </si>
+  <si>
+    <t>1197460105</t>
+  </si>
+  <si>
+    <t>36854</t>
+  </si>
+  <si>
+    <t>CBFSDOJO@testmail.com</t>
+  </si>
+  <si>
+    <t>73164</t>
+  </si>
+  <si>
+    <t>1306698380</t>
+  </si>
+  <si>
+    <t>90535</t>
+  </si>
+  <si>
+    <t>DUQL50SX@testmail.com</t>
+  </si>
+  <si>
+    <t>71620</t>
+  </si>
+  <si>
+    <t>1935491711</t>
+  </si>
+  <si>
+    <t>20112</t>
+  </si>
+  <si>
+    <t>0C6Y6RQN@testmail.com</t>
+  </si>
+  <si>
+    <t>11484</t>
+  </si>
+  <si>
+    <t>1630656925</t>
+  </si>
+  <si>
+    <t>69919</t>
+  </si>
+  <si>
+    <t>334DWD7E@testmail.com</t>
+  </si>
+  <si>
+    <t>33268</t>
+  </si>
+  <si>
+    <t>1259877314</t>
+  </si>
+  <si>
+    <t>41892</t>
+  </si>
+  <si>
+    <t>YHXTCDP1@testmail.com</t>
+  </si>
+  <si>
+    <t>14862</t>
+  </si>
+  <si>
+    <t>1971059754</t>
+  </si>
+  <si>
+    <t>20413</t>
+  </si>
+  <si>
+    <t>HHJ7TGZ4@testmail.com</t>
+  </si>
+  <si>
+    <t>79629</t>
+  </si>
+  <si>
+    <t>1831672394</t>
+  </si>
+  <si>
+    <t>64015</t>
+  </si>
+  <si>
+    <t>XL2UV568@testmail.com</t>
+  </si>
+  <si>
+    <t>46060</t>
+  </si>
+  <si>
+    <t>1355870395</t>
+  </si>
+  <si>
+    <t>90809</t>
+  </si>
+  <si>
+    <t>8IAGAA86@testmail.com</t>
+  </si>
+  <si>
+    <t>48588</t>
+  </si>
+  <si>
+    <t>1931774627</t>
+  </si>
+  <si>
+    <t>27988</t>
+  </si>
+  <si>
+    <t>GIQKVG9Y@testmail.com</t>
+  </si>
+  <si>
+    <t>50836</t>
+  </si>
+  <si>
+    <t>1159795927</t>
+  </si>
+  <si>
+    <t>83623</t>
+  </si>
+  <si>
+    <t>1LYDZ3F7@testmail.com</t>
+  </si>
+  <si>
+    <t>46128</t>
+  </si>
+  <si>
+    <t>1187334222</t>
+  </si>
+  <si>
+    <t>81809</t>
+  </si>
+  <si>
+    <t>TJ30QYYP@testmail.com</t>
+  </si>
+  <si>
+    <t>33602</t>
+  </si>
+  <si>
+    <t>1772766936</t>
+  </si>
+  <si>
+    <t>21264</t>
+  </si>
+  <si>
+    <t>3Z2PJN9L@testmail.com</t>
+  </si>
+  <si>
+    <t>71100</t>
+  </si>
+  <si>
+    <t>1699025943</t>
+  </si>
+  <si>
+    <t>50222</t>
+  </si>
+  <si>
+    <t>JUTK8YMV@testmail.com</t>
+  </si>
+  <si>
+    <t>52765</t>
+  </si>
+  <si>
+    <t>1215577959</t>
+  </si>
+  <si>
+    <t>83210</t>
+  </si>
+  <si>
+    <t>7IXYJFHE@testmail.com</t>
+  </si>
+  <si>
+    <t>33870</t>
+  </si>
+  <si>
+    <t>1534758411</t>
+  </si>
+  <si>
+    <t>21320</t>
+  </si>
+  <si>
+    <t>3H1OACDQ@testmail.com</t>
+  </si>
+  <si>
+    <t>57095</t>
+  </si>
+  <si>
+    <t>1525507756</t>
+  </si>
+  <si>
+    <t>71145</t>
+  </si>
+  <si>
+    <t>0M82CY92@testmail.com</t>
+  </si>
+  <si>
+    <t>60307</t>
+  </si>
+  <si>
+    <t>1259630638</t>
+  </si>
+  <si>
+    <t>17172</t>
+  </si>
+  <si>
+    <t>WKGFKFLD@testmail.com</t>
+  </si>
+  <si>
+    <t>99441</t>
+  </si>
+  <si>
+    <t>1038202514</t>
+  </si>
+  <si>
+    <t>20427</t>
+  </si>
+  <si>
+    <t>AT8G3AZT@testmail.com</t>
+  </si>
+  <si>
+    <t>35358</t>
+  </si>
+  <si>
+    <t>1781465293</t>
+  </si>
+  <si>
+    <t>34980</t>
+  </si>
+  <si>
+    <t>1598IL61@testmail.com</t>
+  </si>
+  <si>
+    <t>18960</t>
+  </si>
+  <si>
+    <t>1694083677</t>
+  </si>
+  <si>
+    <t>32054</t>
+  </si>
+  <si>
+    <t>OZJGL94W@testmail.com</t>
+  </si>
+  <si>
+    <t>51168</t>
+  </si>
+  <si>
+    <t>1887775936</t>
+  </si>
+  <si>
+    <t>11613</t>
+  </si>
+  <si>
+    <t>AV3YPEC2@testmail.com</t>
+  </si>
+  <si>
+    <t>61757</t>
+  </si>
+  <si>
+    <t>1383261546</t>
+  </si>
+  <si>
+    <t>78562</t>
   </si>
 </sst>
 </file>
@@ -637,7 +913,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -932,6 +1208,604 @@
       </c>
       <c r="H11" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+      <c r="G21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>139</v>
+      </c>
+      <c r="E22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>147</v>
+      </c>
+      <c r="E24" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25" t="s">
+        <v>152</v>
+      </c>
+      <c r="F25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" t="s">
+        <v>164</v>
+      </c>
+      <c r="F28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>167</v>
+      </c>
+      <c r="E29" t="s">
+        <v>168</v>
+      </c>
+      <c r="F29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" t="s">
+        <v>172</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>174</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>175</v>
+      </c>
+      <c r="E31" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>179</v>
+      </c>
+      <c r="E32" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>183</v>
+      </c>
+      <c r="E33" t="s">
+        <v>184</v>
+      </c>
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" t="s">
+        <v>188</v>
+      </c>
+      <c r="F34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>